<commit_message>
Add mandatory keywords and fix spelling
Close #2, close #3
</commit_message>
<xml_diff>
--- a/data-raw/metadata/metadata_BEXSTATEST.xlsx
+++ b/data-raw/metadata/metadata_BEXSTATEST.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\STAT\GS\LARPtest\v8\DO_PX\metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\px\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19174995-A6C9-45A3-BD57-3092F2932824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE886CD0-1084-4F6D-8B31-FBF2124313F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20070" windowHeight="11850" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17265" yWindow="0" windowWidth="23220" windowHeight="31800" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables_MD" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="134">
   <si>
     <t>VarName</t>
   </si>
@@ -190,18 +190,9 @@
     <t>UPDATE_FREQUENCY</t>
   </si>
   <si>
-    <t>LAST_UPDATE</t>
-  </si>
-  <si>
     <t>NEXT_UPDATE</t>
   </si>
   <si>
-    <t>DECIMAL</t>
-  </si>
-  <si>
-    <t>SHOWDECIMAL</t>
-  </si>
-  <si>
     <t>LINK_da</t>
   </si>
   <si>
@@ -398,6 +389,42 @@
   </si>
   <si>
     <t>Befolkningsstatistikregistret indeholder …</t>
+  </si>
+  <si>
+    <t>CHARSET</t>
+  </si>
+  <si>
+    <t>utf-8</t>
+  </si>
+  <si>
+    <t>AXIS_VERSION</t>
+  </si>
+  <si>
+    <t>LANGUAGE</t>
+  </si>
+  <si>
+    <t>LANGUAGES</t>
+  </si>
+  <si>
+    <t>MATRIX</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>en","da","kl</t>
+  </si>
+  <si>
+    <t>LAST_UPDATED</t>
+  </si>
+  <si>
+    <t>DECIMALS</t>
+  </si>
+  <si>
+    <t>SHOWDECIMALS</t>
+  </si>
+  <si>
+    <t>BEXSTATEST</t>
   </si>
 </sst>
 </file>
@@ -445,18 +472,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Link 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -474,7 +500,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -802,7 +828,6 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="4"/>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="5" width="30" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
@@ -810,8 +835,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
-      <c r="A1" s="4" t="s">
-        <v>110</v>
+      <c r="A1" t="s">
+        <v>107</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -863,14 +888,14 @@
       <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" t="s">
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
@@ -901,20 +926,20 @@
       </c>
     </row>
     <row r="3" spans="1:15">
-      <c r="A3" s="4" t="s">
-        <v>112</v>
+      <c r="A3" t="s">
+        <v>109</v>
       </c>
       <c r="B3" t="s">
         <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F3" t="s">
         <v>15</v>
@@ -928,14 +953,14 @@
       <c r="I3" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>90</v>
+      <c r="J3" t="s">
+        <v>86</v>
+      </c>
+      <c r="K3" t="s">
+        <v>85</v>
+      </c>
+      <c r="L3" t="s">
+        <v>87</v>
       </c>
       <c r="M3" t="s">
         <v>14</v>
@@ -948,20 +973,20 @@
       </c>
     </row>
     <row r="4" spans="1:15">
-      <c r="A4" s="4" t="s">
-        <v>113</v>
+      <c r="A4" t="s">
+        <v>110</v>
       </c>
       <c r="B4" t="s">
         <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F4" t="s">
         <v>15</v>
@@ -975,14 +1000,14 @@
       <c r="I4" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>90</v>
+      <c r="J4" t="s">
+        <v>86</v>
+      </c>
+      <c r="K4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L4" t="s">
+        <v>87</v>
       </c>
       <c r="M4" t="s">
         <v>14</v>
@@ -995,23 +1020,23 @@
       </c>
     </row>
     <row r="5" spans="1:15">
-      <c r="A5" s="4" t="s">
-        <v>111</v>
+      <c r="A5" t="s">
+        <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
@@ -1076,127 +1101,127 @@
         <v>23</v>
       </c>
       <c r="G1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="4" customFormat="1">
-      <c r="A2" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>90</v>
+      <c r="B2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>122</v>
+      <c r="B3" t="s">
+        <v>119</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>123</v>
+      <c r="B4" t="s">
+        <v>120</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="4" customFormat="1">
-      <c r="A5" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>90</v>
+      <c r="B5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="D5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>106</v>
+      <c r="B6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>103</v>
       </c>
       <c r="D6" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E6" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="F6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>107</v>
+      <c r="B7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>104</v>
       </c>
       <c r="D7" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1206,10 +1231,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B32"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1228,257 +1253,297 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" t="s">
-        <v>65</v>
+        <v>124</v>
+      </c>
+      <c r="B3" s="4">
+        <v>2000</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>125</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15" customHeight="1">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15" customHeight="1">
+        <v>126</v>
+      </c>
+      <c r="B5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15" customHeight="1">
+        <v>127</v>
+      </c>
+      <c r="B6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>124</v>
+        <v>28</v>
+      </c>
+      <c r="B7" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" customHeight="1">
       <c r="A10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>31</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15" customHeight="1">
       <c r="A11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>32</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15" customHeight="1">
       <c r="A12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" t="s">
-        <v>70</v>
+        <v>33</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
-        <v>120</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>118</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B23" t="s">
-        <v>119</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B24" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B25" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B27" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>57</v>
-      </c>
-      <c r="B28">
-        <v>0</v>
+        <v>52</v>
+      </c>
+      <c r="B28" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>58</v>
-      </c>
-      <c r="B29">
-        <v>0</v>
+        <v>53</v>
+      </c>
+      <c r="B29" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>59</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>114</v>
+        <v>54</v>
+      </c>
+      <c r="B30" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>60</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>115</v>
+        <v>130</v>
+      </c>
+      <c r="B31" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>61</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>116</v>
+        <v>55</v>
+      </c>
+      <c r="B32" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>131</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>132</v>
+      </c>
+      <c r="B34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>56</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>57</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B30" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="B31" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
-    <hyperlink ref="B32" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="B35" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="B36" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="B37" r:id="rId3" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1503,16 +1568,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:5">

</xml_diff>

<commit_message>
Use VarName for STUB and HEADING and to join metadata sheets
Close #19
</commit_message>
<xml_diff>
--- a/data-raw/metadata/metadata_BEXSTATEST.xlsx
+++ b/data-raw/metadata/metadata_BEXSTATEST.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/672a29ec829a16e8/Dokumenter/GitHub/ProjCore/px/data-raw/metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Ejstrud\Dropbox\repo\px\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{AE886CD0-1084-4F6D-8B31-FBF2124313F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54DCA15A-A387-4874-9C34-D89930C91919}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72DD2B6-B372-45B2-8244-0BD49BB7926D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28545" yWindow="2730" windowWidth="15330" windowHeight="13275" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables_MD" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="141">
   <si>
     <t>VarName</t>
   </si>
@@ -76,12 +76,6 @@
     <t>antal</t>
   </si>
   <si>
-    <t>fsted</t>
-  </si>
-  <si>
-    <t>sex</t>
-  </si>
-  <si>
     <t>code</t>
   </si>
   <si>
@@ -245,9 +239,6 @@
   </si>
   <si>
     <t>Annually</t>
-  </si>
-  <si>
-    <t>taar</t>
   </si>
   <si>
     <t>time</t>
@@ -512,7 +503,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Link 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -529,12 +520,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -856,11 +843,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="5" width="30" customWidth="1"/>
@@ -870,7 +857,7 @@
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -917,7 +904,7 @@
     </row>
     <row r="2" spans="1:15">
       <c r="B2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
         <v>16</v>
@@ -926,10 +913,10 @@
         <v>16</v>
       </c>
       <c r="E2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G2" t="s">
         <v>14</v>
@@ -961,66 +948,66 @@
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F3" t="s">
         <v>15</v>
       </c>
       <c r="G3" t="s">
+        <v>135</v>
+      </c>
+      <c r="H3" t="s">
+        <v>135</v>
+      </c>
+      <c r="I3" t="s">
+        <v>135</v>
+      </c>
+      <c r="J3" t="s">
+        <v>83</v>
+      </c>
+      <c r="K3" t="s">
+        <v>82</v>
+      </c>
+      <c r="L3" t="s">
+        <v>84</v>
+      </c>
+      <c r="M3" t="s">
         <v>138</v>
       </c>
-      <c r="H3" t="s">
-        <v>138</v>
-      </c>
-      <c r="I3" t="s">
-        <v>138</v>
-      </c>
-      <c r="J3" t="s">
-        <v>86</v>
-      </c>
-      <c r="K3" t="s">
-        <v>85</v>
-      </c>
-      <c r="L3" t="s">
-        <v>87</v>
-      </c>
-      <c r="M3" t="s">
-        <v>141</v>
-      </c>
       <c r="N3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="O3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F4" t="s">
         <v>15</v>
@@ -1035,13 +1022,13 @@
         <v>14</v>
       </c>
       <c r="J4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="K4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="L4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="M4" t="s">
         <v>14</v>
@@ -1055,22 +1042,22 @@
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
@@ -1103,11 +1090,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
@@ -1120,142 +1107,142 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" t="s">
-        <v>23</v>
-      </c>
       <c r="G1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D2" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="F5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="B6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F6" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E7" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F7" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1271,31 +1258,31 @@
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="41.59765625" customWidth="1"/>
-    <col min="2" max="2" width="42.6640625" customWidth="1"/>
+    <col min="1" max="1" width="41.5703125" customWidth="1"/>
+    <col min="2" max="2" width="42.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B3" s="4">
         <v>2000</v>
@@ -1303,263 +1290,263 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" t="s">
         <v>125</v>
-      </c>
-      <c r="B4" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" t="s">
         <v>126</v>
-      </c>
-      <c r="B5" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B6" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>134</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" customHeight="1">
       <c r="A13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15" customHeight="1">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15" customHeight="1">
       <c r="A15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B21" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B25" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B26" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B29" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B30" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B31" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B32" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B33" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B34" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B35" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -1567,7 +1554,7 @@
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -1575,34 +1562,34 @@
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B41" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1621,7 +1608,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="8" customWidth="1"/>
@@ -1634,16 +1621,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:5">

</xml_diff>